<commit_message>
Add ligand data and solvent export script
- Introduced new ligand JSON files for various ligands including DavePhos, DifluorPhos, H8-BINAP, JOSIPHOS, JohnPhos, Me4tBuXPhos, MeO-BIPHEP, MePhos, MorDalPhos, P(2-furyl)3, P(C6F5)3, P(iPr)3, P(mes)3, P(nBu)3, P(o-MeO-Ph)3, P(o-tol)3, P(p-CF3-Ph)3, P(p-Cl-Ph)3, P(p-F-Ph)3, P(p-MeO-Ph)3, P(p-tol)3, PCy3, PEt3, PMe2Ph, PMe3, PMePh2, PPh3, Ph-XPhos, PtBu3, QPhos, RuPhos, SEGPHOS, SPhos, SynPhos, TangPhos, Tol-BINAP, XPhos, XantPhos, tBuBrettPhos, and tBuXPhos.
- Each ligand file contains properties such as cone angle, electronic parameter, bite angle, steric bulk, donor pKa, price category, coordination mode, reaction compatibility, and typical applications.
- Added a backup of the solvents JSON file.
- Implemented a script to export solvent data into a structured JSON format, including properties like dielectric constant, polarity index, boiling point, density, dipole moment, donor number, and reaction compatibility.
</commit_message>
<xml_diff>
--- a/solvent_database.xlsx
+++ b/solvent_database.xlsx
@@ -668,15 +668,11 @@
       <c r="G5" t="n">
         <v>0.8764999999999999</v>
       </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
         <v>0.1</v>
       </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
+      <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
           <t>0.7,0.5,0.2,0.8,0.7</t>
@@ -860,15 +856,9 @@
       <c r="G9" t="n">
         <v>1.594</v>
       </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
           <t>0.3,0.3,0.8,0.4,0.4</t>
@@ -956,15 +946,9 @@
       <c r="G11" t="n">
         <v>0.7781</v>
       </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
           <t>0.4,0.6,0.6,0.5,0.5</t>
@@ -1058,9 +1042,7 @@
       <c r="I13" t="n">
         <v>19.2</v>
       </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
           <t>0.7,0.5,0.5,0.6,0.6</t>
@@ -1106,9 +1088,7 @@
       <c r="I14" t="n">
         <v>26.6</v>
       </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
+      <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
           <t>0.9,0.7,0.2,0.8,0.9</t>
@@ -1154,9 +1134,7 @@
       <c r="I15" t="n">
         <v>29.8</v>
       </c>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
+      <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
           <t>0.8,0.3,0.2,0.9,0.8</t>
@@ -1250,9 +1228,7 @@
       <c r="I17" t="n">
         <v>17.1</v>
       </c>
-      <c r="J17" t="n">
-        <v>0</v>
-      </c>
+      <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr">
         <is>
           <t>0.7,0.4,0.4,0.6,0.8</t>
@@ -1295,12 +1271,8 @@
       <c r="H18" t="n">
         <v>0.08</v>
       </c>
-      <c r="I18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0</v>
-      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
           <t>0.3,0.5,0.6,0.4,0.4</t>
@@ -1490,9 +1462,7 @@
       <c r="I22" t="n">
         <v>33.1</v>
       </c>
-      <c r="J22" t="n">
-        <v>0</v>
-      </c>
+      <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
           <t>0.7,0.6,0.2,0.8,0.7</t>
@@ -1538,9 +1508,7 @@
       <c r="I23" t="n">
         <v>20</v>
       </c>
-      <c r="J23" t="n">
-        <v>0</v>
-      </c>
+      <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr">
         <is>
           <t>0.9,0.6,0.3,0.8,0.8</t>
@@ -1586,9 +1554,7 @@
       <c r="I24" t="n">
         <v>0.1</v>
       </c>
-      <c r="J24" t="n">
-        <v>0</v>
-      </c>
+      <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr">
         <is>
           <t>0.7,0.5,0.2,0.8,0.7</t>
@@ -1679,12 +1645,8 @@
       <c r="H26" t="n">
         <v>0.37</v>
       </c>
-      <c r="I26" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" t="n">
-        <v>0</v>
-      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
           <t>0.7,0.5,0.2,0.8,0.7</t>
@@ -1727,12 +1689,8 @@
       <c r="H27" t="n">
         <v>0.45</v>
       </c>
-      <c r="I27" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" t="n">
-        <v>0</v>
-      </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr">
         <is>
           <t>0.7,0.5,0.2,0.8,0.7</t>
@@ -1775,12 +1733,8 @@
       <c r="H28" t="n">
         <v>0.3</v>
       </c>
-      <c r="I28" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" t="n">
-        <v>0</v>
-      </c>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
           <t>0.7,0.5,0.2,0.8,0.7</t>
@@ -1823,9 +1777,7 @@
       <c r="H29" t="n">
         <v>1.86</v>
       </c>
-      <c r="I29" t="n">
-        <v>0</v>
-      </c>
+      <c r="I29" t="inlineStr"/>
       <c r="J29" t="n">
         <v>0.1</v>
       </c>
@@ -1874,9 +1826,7 @@
       <c r="I30" t="n">
         <v>14.8</v>
       </c>
-      <c r="J30" t="n">
-        <v>0</v>
-      </c>
+      <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr">
         <is>
           <t>0.8,0.6,0.3,0.7,0.8</t>
@@ -1922,9 +1872,7 @@
       <c r="I31" t="n">
         <v>3.3</v>
       </c>
-      <c r="J31" t="n">
-        <v>0</v>
-      </c>
+      <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr">
         <is>
           <t>0.6,0.5,0.2,0.7,0.6</t>
@@ -1970,9 +1918,7 @@
       <c r="I32" t="n">
         <v>16.1</v>
       </c>
-      <c r="J32" t="n">
-        <v>0</v>
-      </c>
+      <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr">
         <is>
           <t>0.6,0.3,0.4,0.5,0.7</t>
@@ -2018,9 +1964,7 @@
       <c r="I33" t="n">
         <v>20.2</v>
       </c>
-      <c r="J33" t="n">
-        <v>0</v>
-      </c>
+      <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr">
         <is>
           <t>0.6,0.5,0.5,0.5,0.6</t>
@@ -2066,9 +2010,7 @@
       <c r="I34" t="n">
         <v>19.5</v>
       </c>
-      <c r="J34" t="n">
-        <v>0</v>
-      </c>
+      <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr">
         <is>
           <t>0.7,0.5,0.5,0.6,0.6</t>
@@ -2156,15 +2098,9 @@
       <c r="G36" t="n">
         <v>0.6840000000000001</v>
       </c>
-      <c r="H36" t="n">
-        <v>0</v>
-      </c>
-      <c r="I36" t="n">
-        <v>0</v>
-      </c>
-      <c r="J36" t="n">
-        <v>0</v>
-      </c>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr">
         <is>
           <t>0.3,0.5,0.6,0.4,0.4</t>
@@ -2258,9 +2194,7 @@
       <c r="I38" t="n">
         <v>16.8</v>
       </c>
-      <c r="J38" t="n">
-        <v>0</v>
-      </c>
+      <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr">
         <is>
           <t>0.7,0.4,0.4,0.6,0.8</t>
@@ -2306,9 +2240,7 @@
       <c r="I39" t="n">
         <v>17.4</v>
       </c>
-      <c r="J39" t="n">
-        <v>0</v>
-      </c>
+      <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr">
         <is>
           <t>0.7,0.3,0.4,0.6,0.8</t>
@@ -2354,9 +2286,7 @@
       <c r="I40" t="n">
         <v>27.3</v>
       </c>
-      <c r="J40" t="n">
-        <v>0</v>
-      </c>
+      <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr">
         <is>
           <t>0.9,0.6,0.2,0.8,0.9</t>
@@ -2435,24 +2365,16 @@
       <c r="D42" t="n">
         <v>1.84</v>
       </c>
-      <c r="E42" t="n">
-        <v>0</v>
-      </c>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="n">
         <v>36.1</v>
       </c>
       <c r="G42" t="n">
         <v>0.626</v>
       </c>
-      <c r="H42" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" t="n">
-        <v>0</v>
-      </c>
-      <c r="J42" t="n">
-        <v>0</v>
-      </c>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr">
         <is>
           <t>0.3,0.5,0.6,0.4,0.4</t>
@@ -2540,15 +2462,9 @@
       <c r="G44" t="n">
         <v>1.622</v>
       </c>
-      <c r="H44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J44" t="n">
-        <v>0</v>
-      </c>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr">
         <is>
           <t>0.4,0.3,0.7,0.5,0.5</t>
@@ -2594,9 +2510,7 @@
       <c r="I45" t="n">
         <v>61</v>
       </c>
-      <c r="J45" t="n">
-        <v>0</v>
-      </c>
+      <c r="J45" t="inlineStr"/>
       <c r="K45" t="inlineStr">
         <is>
           <t>0.8,0.2,0.1,0.9,0.6</t>
@@ -2690,9 +2604,7 @@
       <c r="I47" t="n">
         <v>16.9</v>
       </c>
-      <c r="J47" t="n">
-        <v>0</v>
-      </c>
+      <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr">
         <is>
           <t>0.7,0.4,0.4,0.6,0.8</t>
@@ -2834,9 +2746,7 @@
       <c r="I50" t="n">
         <v>18</v>
       </c>
-      <c r="J50" t="n">
-        <v>0</v>
-      </c>
+      <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr">
         <is>
           <t>0.9,0.6,0.3,0.8,0.8</t>
@@ -2882,9 +2792,7 @@
       <c r="I51" t="n">
         <v>16.5</v>
       </c>
-      <c r="J51" t="n">
-        <v>0</v>
-      </c>
+      <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr">
         <is>
           <t>0.8,0.5,0.4,0.7,0.7</t>
@@ -2930,9 +2838,7 @@
       <c r="I52" t="n">
         <v>14.3</v>
       </c>
-      <c r="J52" t="n">
-        <v>0</v>
-      </c>
+      <c r="J52" t="inlineStr"/>
       <c r="K52" t="inlineStr">
         <is>
           <t>0.7,0.3,0.4,0.6,0.8</t>

</xml_diff>